<commit_message>
Added MG to medical specialty.
</commit_message>
<xml_diff>
--- a/static/fields/deviceclass_reference.xlsx
+++ b/static/fields/deviceclass_reference.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B590A86F-EE82-5A41-9579-44604251D5E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13540" yWindow="760" windowWidth="21880" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="6920" yWindow="760" windowWidth="21880" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -117,6 +123,56 @@
 Value is one of the following
 Y = Device is implantable
 N = Device is not implantable</t>
+  </si>
+  <si>
+    <t>Same as above but with the codes replaced with a human readable description. Note that &amp; and and have been removed from the descriptions as they conflicted with the API syntax).
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
+  <si>
+    <t>device_name</t>
+  </si>
+  <si>
+    <t>This is the proprietary name, or trade name, of the cleared device
+This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>review_panel</t>
+  </si>
+  <si>
+    <t>A three-letter identifier assigned to a device category. Assignment is based upon the medical device classification designated under 21 CFR Parts 862-892, and the technology and intended use of the device. Occasionally these codes are changed over time.</t>
+  </si>
+  <si>
+    <t>Known as the “510(k) Review Panel” since 2014, this helps define the review division within CDRH in which the 510(k) would be reviewed, if it were reviewed today; this is derived from the procode and is always the same as the “Review Advisory Committee” field in the 510(k) database.</t>
+  </si>
+  <si>
+    <t>unclassified_reason</t>
+  </si>
+  <si>
+    <t>This indicates the reason why a device is unclassified (e.g. Pre-Amendment).
+Value is one of the following
+1 = Pre-Amendment
+2 = IDE
+3 = For Export Only
+4 = Unknown
+5 = Guidance Under Development
+6 = Enforcement Discretion
+7 = Not FDA Regulated</t>
+  </si>
+  <si>
+    <t>gmp_exempt_flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+An indication the device is exempt from Good Manufacturing Processes CFR 820. U.S. zip code of the Applicant. See here for more detail.
+Value is one of the following
+Y = Exempt due to Good Manufacturing Practice (GMP)/Quality System
+N = Not exempt due to Good Manufacturing Practice (GMP)/Quality System</t>
+  </si>
+  <si>
+    <t>Facility identifier assigned to facility by the FDA Office of Regulatory Affairs. The openfda section of each document is determined by looking at the product_code value.</t>
   </si>
   <si>
     <t>Regulation Medical Specialty is assigned based on the regulation (e.g. 21 CFR Part 888 is Orthopedic Devices) which is why Class 3 devices lack the “Regulation Medical Specialty” field. Two letters indicating the medical specialty panel responsible for reviewing the product. See link for further detail.
@@ -130,6 +186,7 @@
 HO = General Hospital
 HE = Hematology
 IM = Immunology
+MG = Medical Genetics
 MI = Microbiology
 NE = Neurology
 OB = Obstetrics/Gynecology
@@ -141,61 +198,11 @@
 SU = General, Plastic Surgery
 TX = Clinical Toxicology</t>
   </si>
-  <si>
-    <t>Same as above but with the codes replaced with a human readable description. Note that &amp; and and have been removed from the descriptions as they conflicted with the API syntax).
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>device_name</t>
-  </si>
-  <si>
-    <t>This is the proprietary name, or trade name, of the cleared device
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.</t>
-  </si>
-  <si>
-    <t>product_code</t>
-  </si>
-  <si>
-    <t>review_panel</t>
-  </si>
-  <si>
-    <t>A three-letter identifier assigned to a device category. Assignment is based upon the medical device classification designated under 21 CFR Parts 862-892, and the technology and intended use of the device. Occasionally these codes are changed over time.</t>
-  </si>
-  <si>
-    <t>Known as the “510(k) Review Panel” since 2014, this helps define the review division within CDRH in which the 510(k) would be reviewed, if it were reviewed today; this is derived from the procode and is always the same as the “Review Advisory Committee” field in the 510(k) database.</t>
-  </si>
-  <si>
-    <t>unclassified_reason</t>
-  </si>
-  <si>
-    <t>This indicates the reason why a device is unclassified (e.g. Pre-Amendment).
-Value is one of the following
-1 = Pre-Amendment
-2 = IDE
-3 = For Export Only
-4 = Unknown
-5 = Guidance Under Development
-6 = Enforcement Discretion
-7 = Not FDA Regulated</t>
-  </si>
-  <si>
-    <t>gmp_exempt_flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-An indication the device is exempt from Good Manufacturing Processes CFR 820. U.S. zip code of the Applicant. See here for more detail.
-Value is one of the following
-Y = Exempt due to Good Manufacturing Practice (GMP)/Quality System
-N = Not exempt due to Good Manufacturing Practice (GMP)/Quality System</t>
-  </si>
-  <si>
-    <t>Facility identifier assigned to facility by the FDA Office of Regulatory Affairs. The openfda section of each document is determined by looking at the product_code value.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -709,6 +716,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1033,26 +1048,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="111" style="5" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1066,7 +1079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="105">
+    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1077,7 +1090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="90">
+    <row r="3" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1088,7 +1101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
@@ -1099,7 +1112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1110,7 +1123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="120">
+    <row r="6" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1118,7 +1131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90">
+    <row r="7" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1129,7 +1142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="90">
+    <row r="8" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1140,7 +1153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="360">
+    <row r="9" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
@@ -1148,10 +1161,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1159,10 +1172,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1173,62 +1186,62 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45">
+    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="B14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
+    <row r="15" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="150">
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="90">
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30">
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1239,10 +1252,10 @@
         <v>6</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -1255,8 +1268,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="21" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="42" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Added `summary_malfunction_reporting` field to the Device Classification dataset. Related to https://github.com/FDA/openfda/issues/160
</commit_message>
<xml_diff>
--- a/static/fields/deviceclass_reference.xlsx
+++ b/static/fields/deviceclass_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA8D8DF-8814-354A-8B84-B4E100A78C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6815D44-EF27-6140-AC0A-C3DDC157A8ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="760" windowWidth="21880" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="38340" windowHeight="20120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Field Name</t>
   </si>
@@ -203,6 +203,14 @@
 U = Unclassified
 N = Not classified
 F = HDE</t>
+  </si>
+  <si>
+    <t>summary_malfunction_reporting</t>
+  </si>
+  <si>
+    <t>The Voluntary Malfunction Summary Reporting Program allows participating companies to submit certain medical device malfunction reports in summary form on a quarterly basis.  The program applies to eligible devices regulated by the Center for Devices and Radiological Health (CDRH) and Center for Biologics Evaluation and Research (CBER), including device-led combination products.Value is one of the following:
+Eligible = 510(K)
+Ineligible = PMA</t>
   </si>
 </sst>
 </file>
@@ -1058,16 +1066,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111" style="5" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
@@ -1131,146 +1139,157 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+    <row r="12" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="170" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+    <row r="16" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="119" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
+    <row r="17" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added `summary_malfunction_reporting` field to the Device Classification dataset. Related to https://github.com/FDA/openfda/issues/160 (#206)
</commit_message>
<xml_diff>
--- a/static/fields/deviceclass_reference.xlsx
+++ b/static/fields/deviceclass_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA8D8DF-8814-354A-8B84-B4E100A78C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6815D44-EF27-6140-AC0A-C3DDC157A8ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="760" windowWidth="21880" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="38340" windowHeight="20120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Field Name</t>
   </si>
@@ -203,6 +203,14 @@
 U = Unclassified
 N = Not classified
 F = HDE</t>
+  </si>
+  <si>
+    <t>summary_malfunction_reporting</t>
+  </si>
+  <si>
+    <t>The Voluntary Malfunction Summary Reporting Program allows participating companies to submit certain medical device malfunction reports in summary form on a quarterly basis.  The program applies to eligible devices regulated by the Center for Devices and Radiological Health (CDRH) and Center for Biologics Evaluation and Research (CBER), including device-led combination products.Value is one of the following:
+Eligible = 510(K)
+Ineligible = PMA</t>
   </si>
 </sst>
 </file>
@@ -1058,16 +1066,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="111" style="5" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
@@ -1131,146 +1139,157 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+    <row r="12" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="170" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+    <row r="16" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="119" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
+    <row r="17" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>